<commit_message>
Initial commit of excel_template project
</commit_message>
<xml_diff>
--- a/results_data/empty_book.xlsx
+++ b/results_data/empty_book.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
   <si>
     <t xml:space="preserve">Відбір за виручкою
 Мінімальна середня виручка (тис) = 
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Вибірка зіставних компаній</t>
+  </si>
+  <si>
+    <t>Результати дослідження діяльності обраних компаній за інформацією, отриманою з мережі Інтернет, та додаткової перевірки незалежності компаній</t>
   </si>
 </sst>
 </file>
@@ -97,7 +100,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -136,15 +139,6 @@
       <diagonal/>
     </border>
     <border>
-      <left>
-        <color rgb="00E7EBF7"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="00FFFFFF"/>
       </left>
@@ -163,7 +157,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -174,10 +168,7 @@
     <xf applyAlignment="1" borderId="2" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="3" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="4" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="3" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -192,7 +183,7 @@
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
-      <col>2</col>
+      <col>1</col>
       <colOff>0</colOff>
       <row>0</row>
       <rowOff>0</rowOff>
@@ -576,28 +567,28 @@
     <col customWidth="1" max="5" min="5" width="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row customHeight="1" ht="13" r="1" spans="1:5">
       <c r="A1" s="1" t="n"/>
       <c r="B1" s="1" t="n"/>
       <c r="C1" s="1" t="n"/>
       <c r="D1" s="1" t="n"/>
       <c r="E1" s="1" t="n"/>
     </row>
-    <row r="2" spans="1:5">
+    <row customHeight="1" ht="13" r="2" spans="1:5">
       <c r="A2" s="1" t="n"/>
       <c r="B2" s="1" t="n"/>
       <c r="C2" s="1" t="n"/>
       <c r="D2" s="1" t="n"/>
       <c r="E2" s="1" t="n"/>
     </row>
-    <row customHeight="1" ht="30" r="3" spans="1:5">
+    <row customHeight="1" ht="13" r="3" spans="1:5">
       <c r="A3" s="1" t="n"/>
       <c r="B3" s="1" t="n"/>
       <c r="C3" s="1" t="n"/>
       <c r="D3" s="1" t="n"/>
       <c r="E3" s="1" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="4" spans="1:5">
+    <row customHeight="1" ht="30" r="4" spans="1:5">
       <c r="A4" s="2" t="n"/>
       <c r="B4" s="2" t="n"/>
       <c r="C4" s="2" t="n"/>
@@ -605,25 +596,31 @@
       <c r="E4" s="2" t="n"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="3" t="n"/>
+      <c r="A5" s="3" t="n">
+        <v>1</v>
+      </c>
       <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="4" t="n"/>
+      <c r="C5" s="3" t="n"/>
       <c r="D5" s="3" t="n"/>
       <c r="E5" s="3" t="n"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="3" t="n"/>
+      <c r="A6" s="3" t="n">
+        <v>2</v>
+      </c>
       <c r="B6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="4" t="n"/>
+      <c r="C6" s="3" t="n"/>
       <c r="D6" s="3" t="n"/>
       <c r="E6" s="3" t="n"/>
     </row>
     <row customHeight="1" ht="20" r="7" spans="1:5">
-      <c r="A7" s="3" t="n"/>
+      <c r="A7" s="3" t="n">
+        <v>3</v>
+      </c>
       <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
@@ -632,7 +629,9 @@
       <c r="E7" s="3" t="n"/>
     </row>
     <row customHeight="1" ht="20" r="8" spans="1:5">
-      <c r="A8" s="3" t="n"/>
+      <c r="A8" s="3" t="n">
+        <v>4</v>
+      </c>
       <c r="B8" s="3" t="s">
         <v>3</v>
       </c>
@@ -641,7 +640,9 @@
       <c r="E8" s="3" t="n"/>
     </row>
     <row customHeight="1" ht="20" r="9" spans="1:5">
-      <c r="A9" s="3" t="n"/>
+      <c r="A9" s="3" t="n">
+        <v>5</v>
+      </c>
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
@@ -650,7 +651,9 @@
       <c r="E9" s="3" t="n"/>
     </row>
     <row customHeight="1" ht="20" r="10" spans="1:5">
-      <c r="A10" s="3" t="n"/>
+      <c r="A10" s="3" t="n">
+        <v>6</v>
+      </c>
       <c r="B10" s="3" t="s">
         <v>5</v>
       </c>
@@ -659,7 +662,9 @@
       <c r="E10" s="3" t="n"/>
     </row>
     <row customHeight="1" ht="20" r="11" spans="1:5">
-      <c r="A11" s="3" t="n"/>
+      <c r="A11" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="B11" s="3" t="s">
         <v>6</v>
       </c>
@@ -668,7 +673,9 @@
       <c r="E11" s="3" t="n"/>
     </row>
     <row customHeight="1" ht="20" r="12" spans="1:5">
-      <c r="A12" s="3" t="n"/>
+      <c r="A12" s="3" t="n">
+        <v>8</v>
+      </c>
       <c r="B12" s="3" t="s">
         <v>7</v>
       </c>
@@ -677,7 +684,9 @@
       <c r="E12" s="3" t="n"/>
     </row>
     <row customHeight="1" ht="20" r="13" spans="1:5">
-      <c r="A13" s="3" t="n"/>
+      <c r="A13" s="3" t="n">
+        <v>9</v>
+      </c>
       <c r="B13" s="3" t="s">
         <v>8</v>
       </c>
@@ -686,10 +695,12 @@
       <c r="E13" s="3" t="n"/>
     </row>
     <row customHeight="1" ht="30" r="14" spans="1:5">
-      <c r="A14" s="5" t="n"/>
-      <c r="B14" s="5" t="n"/>
-      <c r="D14" s="5" t="n"/>
-      <c r="E14" s="5" t="n"/>
+      <c r="A14" s="4" t="n"/>
+      <c r="B14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="4" t="n"/>
+      <c r="E14" s="4" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>